<commit_message>
OPSK-1628 - fix to test template files
due to a copy error that propagated across them all
</commit_message>
<xml_diff>
--- a/test/fixtures/files/populated_templates/populated-base-samples-template-with-assay-link.xlsx
+++ b/test/fixtures/files/populated_templates/populated-base-samples-template-with-assay-link.xlsx
@@ -914,23 +914,23 @@
     <t>SOP SEEK ID:</t>
   </si>
   <si>
+    <t>http://localhost:3000/projects/9999</t>
+  </si>
+  <si>
+    <t>My Title</t>
+  </si>
+  <si>
+    <t>My Description</t>
+  </si>
+  <si>
     <t>http://localhost:3000/assays/9999</t>
-  </si>
-  <si>
-    <t>http://localhost:3000/projects/9999</t>
-  </si>
-  <si>
-    <t>My Title</t>
-  </si>
-  <si>
-    <t>My Description</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="Times New Roman"/>
@@ -1017,15 +1017,8 @@
       <family val="1"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF0000FF"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1048,12 +1041,6 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -1220,7 +1207,7 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1688,7 +1675,7 @@
   <dimension ref="A2:AMJ19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1731,7 +1718,7 @@
         <v>275</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="28"/>
@@ -1745,7 +1732,7 @@
         <v>276</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E5" s="27"/>
       <c r="F5" s="28"/>
@@ -1758,8 +1745,8 @@
       <c r="B6" s="10" t="s">
         <v>277</v>
       </c>
-      <c r="C6" s="33" t="s">
-        <v>290</v>
+      <c r="C6" s="7" t="s">
+        <v>289</v>
       </c>
       <c r="E6" s="27"/>
       <c r="F6" s="28"/>
@@ -1807,7 +1794,7 @@
         <v>278</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="E10" s="20"/>
       <c r="F10" s="20"/>
@@ -1915,26 +1902,23 @@
     <dataValidation type="custom" allowBlank="1" sqref="C16">
       <formula1>AND(A1&lt;&gt;"propliteral^wksowlv6")</formula1>
     </dataValidation>
+    <dataValidation type="custom" allowBlank="1" sqref="C6">
+      <formula1>AND(A1&lt;&gt;"propliteral^wksowlv7")</formula1>
+    </dataValidation>
     <dataValidation type="custom" allowBlank="1" sqref="C4">
       <formula1>AND(A1&lt;&gt;"propliteral^wksowlv8")</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" sqref="C10">
-      <formula1>AND(B1048576&lt;&gt;"propliteral^wksowlv5")</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" sqref="C6">
-      <formula1>AND(B1&lt;&gt;"propliteral^wksowlv8")</formula1>
-      <formula2>0</formula2>
+      <formula1>AND(A1&lt;&gt;"propliteral^wksowlv9")</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="E7" r:id="rId1" display="Master metadatasheet guide"/>
     <hyperlink ref="C10" r:id="rId2"/>
-    <hyperlink ref="C6" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId4"/>
-  <drawing r:id="rId5"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>